<commit_message>
Added a new script for HBF IIT 17A.
</commit_message>
<xml_diff>
--- a/HBF IT/Daten/BevDE.xlsx
+++ b/HBF IT/Daten/BevDE.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="9150"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12411-0001" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'12411-0001'!$A:$A,'12411-0001'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -42,207 +42,6 @@
     <t>Anzahl</t>
   </si>
   <si>
-    <t>31.12.1950</t>
-  </si>
-  <si>
-    <t>31.12.1951</t>
-  </si>
-  <si>
-    <t>31.12.1952</t>
-  </si>
-  <si>
-    <t>31.12.1953</t>
-  </si>
-  <si>
-    <t>31.12.1954</t>
-  </si>
-  <si>
-    <t>31.12.1955</t>
-  </si>
-  <si>
-    <t>31.12.1956</t>
-  </si>
-  <si>
-    <t>31.12.1957</t>
-  </si>
-  <si>
-    <t>31.12.1958</t>
-  </si>
-  <si>
-    <t>31.12.1959</t>
-  </si>
-  <si>
-    <t>31.12.1960</t>
-  </si>
-  <si>
-    <t>31.12.1961</t>
-  </si>
-  <si>
-    <t>31.12.1962</t>
-  </si>
-  <si>
-    <t>31.12.1963</t>
-  </si>
-  <si>
-    <t>31.12.1964</t>
-  </si>
-  <si>
-    <t>31.12.1965</t>
-  </si>
-  <si>
-    <t>31.12.1966</t>
-  </si>
-  <si>
-    <t>31.12.1967</t>
-  </si>
-  <si>
-    <t>31.12.1968</t>
-  </si>
-  <si>
-    <t>31.12.1969</t>
-  </si>
-  <si>
-    <t>31.12.1970</t>
-  </si>
-  <si>
-    <t>31.12.1971</t>
-  </si>
-  <si>
-    <t>31.12.1972</t>
-  </si>
-  <si>
-    <t>31.12.1973</t>
-  </si>
-  <si>
-    <t>31.12.1974</t>
-  </si>
-  <si>
-    <t>31.12.1975</t>
-  </si>
-  <si>
-    <t>31.12.1976</t>
-  </si>
-  <si>
-    <t>31.12.1977</t>
-  </si>
-  <si>
-    <t>31.12.1978</t>
-  </si>
-  <si>
-    <t>31.12.1979</t>
-  </si>
-  <si>
-    <t>31.12.1980</t>
-  </si>
-  <si>
-    <t>31.12.1981</t>
-  </si>
-  <si>
-    <t>31.12.1982</t>
-  </si>
-  <si>
-    <t>31.12.1983</t>
-  </si>
-  <si>
-    <t>31.12.1984</t>
-  </si>
-  <si>
-    <t>31.12.1985</t>
-  </si>
-  <si>
-    <t>31.12.1986</t>
-  </si>
-  <si>
-    <t>31.12.1987</t>
-  </si>
-  <si>
-    <t>31.12.1988</t>
-  </si>
-  <si>
-    <t>31.12.1989</t>
-  </si>
-  <si>
-    <t>31.12.1990</t>
-  </si>
-  <si>
-    <t>31.12.1991</t>
-  </si>
-  <si>
-    <t>31.12.1992</t>
-  </si>
-  <si>
-    <t>31.12.1993</t>
-  </si>
-  <si>
-    <t>31.12.1994</t>
-  </si>
-  <si>
-    <t>31.12.1995</t>
-  </si>
-  <si>
-    <t>31.12.1996</t>
-  </si>
-  <si>
-    <t>31.12.1997</t>
-  </si>
-  <si>
-    <t>31.12.1998</t>
-  </si>
-  <si>
-    <t>31.12.1999</t>
-  </si>
-  <si>
-    <t>31.12.2000</t>
-  </si>
-  <si>
-    <t>31.12.2001</t>
-  </si>
-  <si>
-    <t>31.12.2002</t>
-  </si>
-  <si>
-    <t>31.12.2003</t>
-  </si>
-  <si>
-    <t>31.12.2004</t>
-  </si>
-  <si>
-    <t>31.12.2005</t>
-  </si>
-  <si>
-    <t>31.12.2006</t>
-  </si>
-  <si>
-    <t>31.12.2007</t>
-  </si>
-  <si>
-    <t>31.12.2008</t>
-  </si>
-  <si>
-    <t>31.12.2009</t>
-  </si>
-  <si>
-    <t>31.12.2010</t>
-  </si>
-  <si>
-    <t>31.12.2011</t>
-  </si>
-  <si>
-    <t>31.12.2012</t>
-  </si>
-  <si>
-    <t>31.12.2013</t>
-  </si>
-  <si>
-    <t>31.12.2014</t>
-  </si>
-  <si>
-    <t>31.12.2015</t>
-  </si>
-  <si>
-    <t>31.12.2016</t>
-  </si>
-  <si>
     <t>__________</t>
   </si>
   <si>
@@ -256,12 +55,213 @@
   </si>
   <si>
     <t>Stand: 11.02.2018 - 16:16:26</t>
+  </si>
+  <si>
+    <t>1950</t>
+  </si>
+  <si>
+    <t>1951</t>
+  </si>
+  <si>
+    <t>1952</t>
+  </si>
+  <si>
+    <t>1953</t>
+  </si>
+  <si>
+    <t>1954</t>
+  </si>
+  <si>
+    <t>1955</t>
+  </si>
+  <si>
+    <t>1956</t>
+  </si>
+  <si>
+    <t>1957</t>
+  </si>
+  <si>
+    <t>1958</t>
+  </si>
+  <si>
+    <t>1959</t>
+  </si>
+  <si>
+    <t>1960</t>
+  </si>
+  <si>
+    <t>1961</t>
+  </si>
+  <si>
+    <t>1962</t>
+  </si>
+  <si>
+    <t>1963</t>
+  </si>
+  <si>
+    <t>1964</t>
+  </si>
+  <si>
+    <t>1965</t>
+  </si>
+  <si>
+    <t>1966</t>
+  </si>
+  <si>
+    <t>1967</t>
+  </si>
+  <si>
+    <t>1968</t>
+  </si>
+  <si>
+    <t>1969</t>
+  </si>
+  <si>
+    <t>1970</t>
+  </si>
+  <si>
+    <t>1971</t>
+  </si>
+  <si>
+    <t>1972</t>
+  </si>
+  <si>
+    <t>1973</t>
+  </si>
+  <si>
+    <t>1974</t>
+  </si>
+  <si>
+    <t>1975</t>
+  </si>
+  <si>
+    <t>1976</t>
+  </si>
+  <si>
+    <t>1977</t>
+  </si>
+  <si>
+    <t>1978</t>
+  </si>
+  <si>
+    <t>1979</t>
+  </si>
+  <si>
+    <t>1980</t>
+  </si>
+  <si>
+    <t>1981</t>
+  </si>
+  <si>
+    <t>1982</t>
+  </si>
+  <si>
+    <t>1983</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>1985</t>
+  </si>
+  <si>
+    <t>1986</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>1988</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -376,9 +376,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -398,6 +395,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -413,6 +413,1326 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Entwicklung</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> dert Bevölkerung in Deutschland</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'12411-0001'!$A$6:$A$72</c:f>
+              <c:strCache>
+                <c:ptCount val="67"/>
+                <c:pt idx="0">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1951</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1952</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1954</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1955</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1956</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1957</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1958</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1959</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1960</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1961</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1962</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1963</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1964</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1965</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1966</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1967</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1968</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1969</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'12411-0001'!$B$6:$B$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="67"/>
+                <c:pt idx="0">
+                  <c:v>50958125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51434777</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51863761</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52453806</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52943295</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53517683</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53339626</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54064365</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54719159</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55257088</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55958321</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56589148</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>57247246</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>57864509</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>58587451</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>59296591</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59792934</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>59948474</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60463033</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>61194591</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>61001164</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>61502503</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>61809378</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>62101369</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>61991475</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>61644624</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>61441996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>61352745</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>61321663</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>61439342</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>61657945</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>61712689</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>61546101</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>61306669</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>61049256</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>61020474</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>61140461</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>61238079</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>61715103</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>62679035</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>79753227</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>80274564</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>80974632</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>81338093</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>81538603</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>81817499</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>82012162</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>82057379</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>82037011</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>82163475</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>82259540</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>82440309</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>82536680</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>82531671</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>82500849</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>82437995</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>82314906</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>82217837</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>82002356</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>81802257</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>81751602</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>80327900</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>80523746</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>80767463</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>81197537</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>82175684</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>82521653</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-624E-4150-93AB-11E86B454841}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="447983384"/>
+        <c:axId val="447983712"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="447983384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-407]mmmmm;@" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="447983712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="447983712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="447983384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438156</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>133356</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{541C5E67-C6F5-4199-82A8-A03FD38AB283}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -711,14 +2031,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:A5"/>
+      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -729,568 +2049,568 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
+      <c r="A6" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>50958125</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>7</v>
+      <c r="A7" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="B7" s="1">
         <v>51434777</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>8</v>
+      <c r="A8" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>51863761</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>9</v>
+      <c r="A9" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <v>52453806</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>10</v>
+      <c r="A10" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="B10" s="1">
         <v>52943295</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>11</v>
+      <c r="A11" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="B11" s="1">
         <v>53517683</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>12</v>
+      <c r="A12" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="B12" s="1">
         <v>53339626</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>13</v>
+      <c r="A13" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="B13" s="1">
         <v>54064365</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>14</v>
+      <c r="A14" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="B14" s="1">
         <v>54719159</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>15</v>
+      <c r="A15" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="B15" s="1">
         <v>55257088</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>16</v>
+      <c r="A16" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="B16" s="1">
         <v>55958321</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>17</v>
+      <c r="A17" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="B17" s="1">
         <v>56589148</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>18</v>
+      <c r="A18" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="B18" s="1">
         <v>57247246</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>19</v>
+      <c r="A19" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B19" s="1">
         <v>57864509</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>20</v>
+      <c r="A20" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="B20" s="1">
         <v>58587451</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>21</v>
+      <c r="A21" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="B21" s="1">
         <v>59296591</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>22</v>
+      <c r="A22" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="B22" s="1">
         <v>59792934</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>23</v>
+      <c r="A23" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="B23" s="1">
         <v>59948474</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>24</v>
+      <c r="A24" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="B24" s="1">
         <v>60463033</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>25</v>
+      <c r="A25" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="B25" s="1">
         <v>61194591</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>26</v>
+      <c r="A26" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>61001164</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>27</v>
+      <c r="A27" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="B27" s="1">
         <v>61502503</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>28</v>
+      <c r="A28" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="B28" s="1">
         <v>61809378</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>29</v>
+      <c r="A29" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="B29" s="1">
         <v>62101369</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>30</v>
+      <c r="A30" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="B30" s="1">
         <v>61991475</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>31</v>
+      <c r="A31" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="B31" s="1">
         <v>61644624</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>32</v>
+      <c r="A32" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="B32" s="1">
         <v>61441996</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>33</v>
+      <c r="A33" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="B33" s="1">
         <v>61352745</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>34</v>
+      <c r="A34" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="B34" s="1">
         <v>61321663</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>35</v>
+      <c r="A35" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="B35" s="1">
         <v>61439342</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>36</v>
+      <c r="A36" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="B36" s="1">
         <v>61657945</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>37</v>
+      <c r="A37" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="B37" s="1">
         <v>61712689</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>38</v>
+      <c r="A38" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="B38" s="1">
         <v>61546101</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>39</v>
+      <c r="A39" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="B39" s="1">
         <v>61306669</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>40</v>
+      <c r="A40" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="B40" s="1">
         <v>61049256</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>41</v>
+      <c r="A41" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="B41" s="1">
         <v>61020474</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>42</v>
+      <c r="A42" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B42" s="1">
         <v>61140461</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>43</v>
+      <c r="A43" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="B43" s="1">
         <v>61238079</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>44</v>
+      <c r="A44" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="B44" s="1">
         <v>61715103</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>45</v>
+      <c r="A45" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="B45" s="1">
         <v>62679035</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>46</v>
+      <c r="A46" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="B46" s="1">
         <v>79753227</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>47</v>
+      <c r="A47" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="B47" s="1">
         <v>80274564</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>48</v>
+      <c r="A48" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="B48" s="1">
         <v>80974632</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>49</v>
+      <c r="A49" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="B49" s="1">
         <v>81338093</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>50</v>
+      <c r="A50" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="B50" s="1">
         <v>81538603</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>51</v>
+      <c r="A51" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="B51" s="1">
         <v>81817499</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>52</v>
+      <c r="A52" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="B52" s="1">
         <v>82012162</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>53</v>
+      <c r="A53" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="B53" s="1">
         <v>82057379</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>54</v>
+      <c r="A54" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="B54" s="1">
         <v>82037011</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>55</v>
+      <c r="A55" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="B55" s="1">
         <v>82163475</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>56</v>
+      <c r="A56" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="B56" s="1">
         <v>82259540</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>57</v>
+      <c r="A57" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="B57" s="1">
         <v>82440309</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>58</v>
+      <c r="A58" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="B58" s="1">
         <v>82536680</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>59</v>
+      <c r="A59" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="B59" s="1">
         <v>82531671</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>60</v>
+      <c r="A60" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="B60" s="1">
         <v>82500849</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>61</v>
+      <c r="A61" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="B61" s="1">
         <v>82437995</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>62</v>
+      <c r="A62" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="B62" s="1">
         <v>82314906</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>63</v>
+      <c r="A63" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="B63" s="1">
         <v>82217837</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>64</v>
+      <c r="A64" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="B64" s="1">
         <v>82002356</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>65</v>
+      <c r="A65" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="B65" s="1">
         <v>81802257</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>66</v>
+      <c r="A66" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="B66" s="1">
         <v>81751602</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>67</v>
+      <c r="A67" s="11" t="s">
+        <v>72</v>
       </c>
       <c r="B67" s="1">
         <v>80327900</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>68</v>
+      <c r="A68" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="B68" s="1">
         <v>80523746</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>69</v>
+      <c r="A69" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="B69" s="1">
         <v>80767463</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>70</v>
+      <c r="A70" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="B70" s="1">
         <v>81197537</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>71</v>
+      <c r="A71" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="B71" s="1">
         <v>82175684</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>72</v>
+      <c r="A72" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="B72" s="1">
         <v>82521653</v>
@@ -1298,27 +2618,27 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1335,5 +2655,6 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CAbruf:11.02.2018 - 16:16:26, Seite &amp;P von &amp;N&amp;L&amp;R</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>